<commit_message>
mudança na formula condicional
</commit_message>
<xml_diff>
--- a/Controle de Metas.xlsx
+++ b/Controle de Metas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\curso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66530161-9922-49AF-B0E2-6EBBA2701E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03127F90-5429-49E0-9C2B-CFECB094645C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6738200-FEEA-4DAF-AC51-5C3509537603}"/>
   </bookViews>
@@ -98,7 +98,154 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -474,11 +621,11 @@
         <v>90</v>
       </c>
       <c r="C2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2">
         <f>C2/B2</f>
-        <v>1</v>
+        <v>0.98888888888888893</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -492,6 +639,15 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+      <formula>$B$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>$B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
formulas copiadas para periodos de metas
</commit_message>
<xml_diff>
--- a/Controle de Metas.xlsx
+++ b/Controle de Metas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\curso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03127F90-5429-49E0-9C2B-CFECB094645C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF177368-7EAF-4469-B07B-C663B6498593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6738200-FEEA-4DAF-AC51-5C3509537603}"/>
   </bookViews>
@@ -89,55 +89,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -163,85 +127,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -555,96 +440,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566436B3-9281-48EF-8CE8-BC164A203AA7}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="N1" sqref="N1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>90</v>
-      </c>
-      <c r="C2">
-        <v>89</v>
-      </c>
-      <c r="D2">
-        <f>C2/B2</f>
-        <v>0.98888888888888893</v>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <v>89</v>
+      </c>
+      <c r="D3">
+        <f>C3/B3</f>
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="E3">
+        <v>90</v>
+      </c>
+      <c r="F3">
+        <v>89</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3" si="0">F3/E3</f>
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+      <c r="I3">
+        <v>89</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3" si="1">I3/H3</f>
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="K3">
+        <v>90</v>
+      </c>
+      <c r="L3">
+        <v>89</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3" si="2">L3/K3</f>
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="N3">
+        <v>90</v>
+      </c>
+      <c r="O3">
+        <v>89</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3" si="3">O3/N3</f>
+        <v>0.98888888888888893</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
-      <formula>$B$2</formula>
+  <mergeCells count="5">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3 I3 L3 O3">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>$B$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
-      <formula>$B$2</formula>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+      <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>$B$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>$B$3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>